<commit_message>
completed extracted encounter script and extracted to intermediary
</commit_message>
<xml_diff>
--- a/summary_files/intersection_locations.xlsx
+++ b/summary_files/intersection_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\01eco\Desktop\UoGuelph\Masters Research Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\01eco\Desktop\UoGuelph\multisource_ML_research\summary_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13729B7C-B5D7-4F45-9DA5-8E1C995CA775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2925A38D-6B8A-4B88-8FF1-DB386AF43AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-13095" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{9C2FDA27-E63F-477C-BD6F-2D7FCA74FFB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{9C2FDA27-E63F-477C-BD6F-2D7FCA74FFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="order_0" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,6 @@
     <t>3_y_ltminor</t>
   </si>
   <si>
-    <t>0_x_half</t>
-  </si>
-  <si>
     <t>0_y_lthalf</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>3_y_ltsig</t>
+  </si>
+  <si>
+    <t>0_x_lthalf</t>
   </si>
 </sst>
 </file>
@@ -640,30 +640,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1090A18D-F34D-4911-87D6-21C346BEE22B}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
       </c>
       <c r="G1" t="s">
         <v>14</v>
@@ -707,7 +707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BDA31D-F390-4805-AD51-72D967D9C7E6}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
@@ -715,28 +715,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1012,20 +1012,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="4ee619da-c3e5-4c95-909e-b5f1aea153a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="4ee619da-c3e5-4c95-909e-b5f1aea153a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1048,14 +1048,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C52CD57-825E-4BCA-B304-2B31D64329B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A27E39F-E0D0-435D-8B0E-10E1B566D481}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1070,4 +1062,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C52CD57-825E-4BCA-B304-2B31D64329B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
renamed file endings changing ltsig to ltsignal. updated headings in intersection_locations
</commit_message>
<xml_diff>
--- a/summary_files/intersection_locations.xlsx
+++ b/summary_files/intersection_locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\01eco\Desktop\UoGuelph\multisource_ML_research\summary_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2925A38D-6B8A-4B88-8FF1-DB386AF43AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DD145D-438D-40C8-A9D6-90DF0278B8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{9C2FDA27-E63F-477C-BD6F-2D7FCA74FFB5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{9C2FDA27-E63F-477C-BD6F-2D7FCA74FFB5}"/>
   </bookViews>
   <sheets>
     <sheet name="order_0" sheetId="1" r:id="rId1"/>
@@ -101,12 +101,6 @@
     <t>1_x_ltminor</t>
   </si>
   <si>
-    <t>2_x_ltsig</t>
-  </si>
-  <si>
-    <t>2_y_ltsig</t>
-  </si>
-  <si>
     <t>0_x_ltminor</t>
   </si>
   <si>
@@ -125,13 +119,19 @@
     <t>2_y_ltmajor</t>
   </si>
   <si>
-    <t>3_x_ltsig</t>
-  </si>
-  <si>
-    <t>3_y_ltsig</t>
-  </si>
-  <si>
     <t>0_x_lthalf</t>
+  </si>
+  <si>
+    <t>2_x_ltsignal</t>
+  </si>
+  <si>
+    <t>2_y_ltsignal</t>
+  </si>
+  <si>
+    <t>3_x_ltsignal</t>
+  </si>
+  <si>
+    <t>3_y_ltsignal</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,15 +640,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1090A18D-F34D-4911-87D6-21C346BEE22B}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
@@ -660,10 +660,10 @@
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
         <v>14</v>
@@ -707,36 +707,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BDA31D-F390-4805-AD51-72D967D9C7E6}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
       <c r="G1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1012,20 +1012,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="4ee619da-c3e5-4c95-909e-b5f1aea153a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="4ee619da-c3e5-4c95-909e-b5f1aea153a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1048,6 +1048,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C52CD57-825E-4BCA-B304-2B31D64329B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A27E39F-E0D0-435D-8B0E-10E1B566D481}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1062,12 +1070,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C52CD57-825E-4BCA-B304-2B31D64329B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>